<commit_message>
next day and create summary data for day
</commit_message>
<xml_diff>
--- a/history/25_35/data_ticker_1703.xlsx
+++ b/history/25_35/data_ticker_1703.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavel.rostov\PycharmProjects\scrapyBotTrade\history\25_35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF24C7ED-17C8-4B06-BECF-3200F812862D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A0463C-9048-431F-AEA8-12A27FFD0408}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28545" yWindow="0" windowWidth="27000" windowHeight="15075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1983,7 +1983,7 @@
   <dimension ref="A1:CR252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CW5" sqref="CW5"/>
+      <selection activeCell="CX9" sqref="CX9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>

</xml_diff>